<commit_message>
Projektdokumentation, Anpassung Phasen, Zeiterfassung
</commit_message>
<xml_diff>
--- a/docs/03 Organisatorisches/Zeiterfassung.xlsx
+++ b/docs/03 Organisatorisches/Zeiterfassung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20235" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20235"/>
   </bookViews>
   <sheets>
     <sheet name="Zeiterfassung" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Datum</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>PSP-Code</t>
+  </si>
+  <si>
+    <t>Brainstorming, telefonat mit Mejdin</t>
+  </si>
+  <si>
+    <t>Mindmap Inputs</t>
+  </si>
+  <si>
+    <t>Initiale Projektdokumentation</t>
   </si>
 </sst>
 </file>
@@ -181,10 +190,10 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -224,8 +233,8 @@
     <tableColumn id="1" name="Tätigkeit" dataDxfId="4"/>
     <tableColumn id="2" name="Wer" dataDxfId="3"/>
     <tableColumn id="3" name="Datum" dataDxfId="2"/>
-    <tableColumn id="5" name="PSP-Code" dataDxfId="0"/>
-    <tableColumn id="4" name="(In Stunden)Zeit" dataDxfId="1"/>
+    <tableColumn id="5" name="PSP-Code" dataDxfId="1"/>
+    <tableColumn id="4" name="(In Stunden)Zeit" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -520,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,8 +587,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>42245</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4">
+        <v>42246</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>42246</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
@@ -667,7 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Anpassungen Zeiterfassung und Phasenplan Organigram
</commit_message>
<xml_diff>
--- a/docs/03 Organisatorisches/Zeiterfassung.xlsx
+++ b/docs/03 Organisatorisches/Zeiterfassung.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Datum</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Initiale Projektdokumentation</t>
+  </si>
+  <si>
+    <t>Pflichtenheft sowie Phasenplan arbeiten</t>
+  </si>
+  <si>
+    <t>Review</t>
   </si>
 </sst>
 </file>
@@ -530,7 +536,7 @@
   <dimension ref="B1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,6 +633,34 @@
       </c>
       <c r="F6" s="1">
         <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4">
+        <v>42249</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>42258</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Grobplanung (ohne effektive Daten, lediglich Aufwandschätzung)
</commit_message>
<xml_diff>
--- a/docs/03 Organisatorisches/Zeiterfassung.xlsx
+++ b/docs/03 Organisatorisches/Zeiterfassung.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Datum</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Review</t>
+  </si>
+  <si>
+    <t>PSP Draf, Ausserorderntliche Planung</t>
+  </si>
+  <si>
+    <t>Grob Planung - Lastenhef Reviews</t>
   </si>
 </sst>
 </file>
@@ -233,8 +239,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B1:F100" totalsRowShown="0" headerRowBorderDxfId="5">
-  <autoFilter ref="B1:F100"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B1:F101" totalsRowShown="0" headerRowBorderDxfId="5">
+  <autoFilter ref="B1:F101"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Tätigkeit" dataDxfId="4"/>
     <tableColumn id="2" name="Wer" dataDxfId="3"/>
@@ -533,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F27"/>
+  <dimension ref="B1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,20 +669,45 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4">
+        <v>42259</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="4">
+        <v>42260</v>
+      </c>
+      <c r="F10" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
@@ -686,6 +717,9 @@
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
     </row>
   </sheetData>
   <sortState ref="B4:E79">
@@ -693,7 +727,7 @@
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C100">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C101">
       <formula1>Entwickler</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Use Case update Zeiterfassung
</commit_message>
<xml_diff>
--- a/docs/03 Organisatorisches/Zeiterfassung.xlsx
+++ b/docs/03 Organisatorisches/Zeiterfassung.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
   <si>
     <t>Datum</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>Lösungsvariante 2 &amp; 3</t>
+  </si>
+  <si>
+    <t>Klassendiagram</t>
+  </si>
+  <si>
+    <t>Java Klassen</t>
+  </si>
+  <si>
+    <t>Use Cases</t>
   </si>
 </sst>
 </file>
@@ -590,7 +599,7 @@
   <dimension ref="B1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,18 +1007,76 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="4">
+        <v>42315</v>
+      </c>
+      <c r="F29" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="4">
+        <v>42316</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="4">
+        <v>42317</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="4">
+        <v>42318</v>
+      </c>
+      <c r="F32" s="1">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="4">
+        <v>42320</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
     </row>
   </sheetData>
@@ -1018,7 +1085,7 @@
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19:D24 C2:C18 C25:C107 D26:D28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19:D24 C2:C18 D26:D28 C25:C107">
       <formula1>Entwickler</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>